<commit_message>
commiting course changes to backlogs and defect table
</commit_message>
<xml_diff>
--- a/doc/projectFiles/ProductBacklog.xlsx
+++ b/doc/projectFiles/ProductBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="801"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$4:$H$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$A$4:$H$21</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -123,27 +123,18 @@
     <t>Filterobjekterstellung</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich verschiedene Darstellungen der analysierten Daten</t>
-  </si>
-  <si>
     <t>Darstellung</t>
   </si>
   <si>
     <t>4-2</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich einzelene Tweets manuell ausblenden, sodass diese nicht analysiert werden</t>
-  </si>
-  <si>
     <t>Funktionalität: Ausblenden</t>
   </si>
   <si>
     <t>4-3</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich einzelene Tweets manuell löschen, sodass diese nicht wieder analysiert werden</t>
-  </si>
-  <si>
     <t>Funktionalität: Löschen</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>1-5</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich über Tweets informiert werden</t>
-  </si>
-  <si>
     <t>Benachrichtigung</t>
   </si>
   <si>
@@ -210,23 +198,41 @@
     <t>3-3</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; will ich eigene Keywords für die positiv / negativ Semtimentanalyse bestimmen können.</t>
-  </si>
-  <si>
     <t>Als &lt;MM&gt; will ich vorhandene Veranstaltungen klonen, um bestimme Parameter zu übernehmen, aber die ursprüngliche Veranstaltung nicht zu verändern.</t>
   </si>
   <si>
-    <t>Als &lt;MM&gt; möchte ich eine Mindestanzahl von zu sammelden Tweets angeben, damit ich bewerten kann, ob das Analyseergebnis sinnvoll ist.</t>
-  </si>
-  <si>
-    <t>Als &lt;MM&gt; will ich zu einer bestimmten Veranstaltung gehörende Daten als .csv exportieren</t>
+    <t>Als &lt;MM&gt; will ich bereits angelegte Filter auch löschen können.</t>
+  </si>
+  <si>
+    <t>5-1</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich eigene Keywords in beliebiger Sprache für die positiv / negativ Semtimentanalyse bestimmen können.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; möchte ich eine Mindestanzahl von zu sammelden Tweets pro Veranstaltung angeben, damit ich bewerten kann, ob das Analyseergebnis sinnvoll ist.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich verschiedene Darstellungen der analysierten Daten.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich einzelene Tweets manuell löschen, sodass diese nicht wieder analysiert werden.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich einzelene Tweets manuell für einen Filter ausblenden, sodass diese nicht analysiert werden.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich zu einer bestimmten Veranstaltung gehörende Daten als .csv exportieren.</t>
+  </si>
+  <si>
+    <t>Als &lt;MM&gt; will ich über Tweets informiert werden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -399,7 +405,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -409,7 +415,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -429,16 +434,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -797,36 +809,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="80.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="1" max="1" width="6" style="22" customWidth="1"/>
+    <col min="2" max="2" width="109.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" ht="23.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -851,231 +866,236 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="3">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
         <v>100</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12">
         <v>60</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>3</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12">
         <v>55</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
         <v>99</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="14" t="s">
+      <c r="G8" s="5"/>
+      <c r="H8" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15">
         <v>55</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18" t="s">
+      <c r="G9" s="16"/>
+      <c r="H9" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="24">
         <v>3</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="E11">
+      <c r="C11" s="26"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="16" t="s">
         <v>32</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="6">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6">
         <v>27</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+      <c r="A14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>40</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
       <c r="E15">
-        <v>15</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16">
         <v>15</v>
@@ -1083,149 +1103,198 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>43</v>
+      <c r="G16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>64</v>
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>11</v>
-      </c>
-      <c r="G17" s="21"/>
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="3"/>
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="3"/>
+      <c r="B23" s="21"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E18">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" t="s">
         <v>10</v>
       </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="3" t="s">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B43" t="s">
         <v>48</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="3" t="s">
+    <row r="44" spans="1:6">
+      <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B44" t="s">
         <v>50</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F44" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="3" t="s">
+    <row r="45" spans="1:6">
+      <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="3" t="s">
+      <c r="C45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="3" t="s">
+      <c r="C46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="F26" s="4" t="s">
+      <c r="C47" s="4"/>
+      <c r="F47" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A4:H20">
-    <sortState ref="A10:H20">
-      <sortCondition descending="1" ref="E4:E20"/>
+  <autoFilter ref="A4:H21">
+    <filterColumn colId="7">
+      <filters blank="1"/>
+    </filterColumn>
+    <sortState ref="A12:H21">
+      <sortCondition descending="1" ref="E4:E21"/>
     </sortState>
   </autoFilter>
   <sortState ref="A5:H27">
@@ -1235,7 +1304,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added Zeitdokumentation und Sprint bei Dokumentation
</commit_message>
<xml_diff>
--- a/doc/projectFiles/ProductBacklog.xlsx
+++ b/doc/projectFiles/ProductBacklog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8205" tabRatio="801"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="801"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -234,8 +234,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -451,8 +451,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -812,24 +812,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" style="21" customWidth="1"/>
     <col min="2" max="2" width="93" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25">
+    <row r="1" spans="1:8" ht="23">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -869,7 +868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -893,7 +892,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -917,7 +916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -941,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -961,7 +960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -981,7 +980,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>60</v>
       </c>
@@ -1044,7 +1043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="18" t="s">
         <v>57</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
         <v>13</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>36</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1125,7 +1124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>41</v>
       </c>
@@ -1313,9 +1312,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:H21">
-    <filterColumn colId="7">
-      <filters blank="1"/>
-    </filterColumn>
     <sortState ref="A12:H21">
       <sortCondition descending="1" ref="E4:E21"/>
     </sortState>
@@ -1337,12 +1333,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1354,12 +1350,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1371,12 +1367,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>